<commit_message>
Se agrega etiqueta neutral
</commit_message>
<xml_diff>
--- a/clasificaciones_preguntas.xlsx
+++ b/clasificaciones_preguntas.xlsx
@@ -477,7 +477,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Positiva</t>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -489,7 +489,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Negativa</t>
+          <t>Positiva</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Positiva</t>
+          <t>Negativa</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Negativa</t>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Positiva</t>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Negativa</t>
+          <t>Positiva</t>
         </is>
       </c>
     </row>
@@ -573,7 +573,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Positiva</t>
+          <t>Negativa</t>
         </is>
       </c>
     </row>
@@ -585,7 +585,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Negativa</t>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Positiva</t>
+          <t>Neutral</t>
         </is>
       </c>
     </row>
@@ -633,7 +633,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Negativa</t>
+          <t>Positiva</t>
         </is>
       </c>
     </row>
@@ -645,7 +645,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Positiva</t>
+          <t>Negativa</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Negativa</t>
+          <t>Neutral</t>
         </is>
       </c>
     </row>

</xml_diff>